<commit_message>
Fixed login logout, profile, changed calendar to timesheet list
</commit_message>
<xml_diff>
--- a/timesheet/excel_files/activities.xlsx
+++ b/timesheet/excel_files/activities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PNB-IT\Documents\code\timesheets_app\docker-timesheets\timesheet\excel_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PNB-IT\Documents\code\timesheets_app_no_docker\timesheets_main\timesheet\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FEF232C-7CEC-442F-A821-D51CFDA2D13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF6BD78-855C-4D9E-B5B9-506E2ED6C1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="1480" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -926,7 +926,7 @@
     <t>code</t>
   </si>
   <si>
-    <t>description</t>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -1326,11 +1326,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="90" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -1340,7 +1343,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1420,7 +1423,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -1484,7 +1487,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="186" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="186" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -1580,7 +1583,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="62" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" ht="62" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
@@ -1740,7 +1743,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>100</v>
       </c>
@@ -1748,7 +1751,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>102</v>
       </c>
@@ -1756,7 +1759,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>104</v>
       </c>
@@ -1764,7 +1767,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="62" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>106</v>
       </c>
@@ -1772,7 +1775,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="62" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>108</v>
       </c>
@@ -1780,7 +1783,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>110</v>
       </c>
@@ -1788,7 +1791,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>112</v>
       </c>
@@ -1796,7 +1799,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>114</v>
       </c>
@@ -1804,7 +1807,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="232.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>116</v>
       </c>
@@ -1812,7 +1815,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="62" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>118</v>
       </c>
@@ -1820,7 +1823,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>120</v>
       </c>
@@ -1828,7 +1831,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>122</v>
       </c>
@@ -1836,7 +1839,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>124</v>
       </c>
@@ -1844,7 +1847,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="124" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>126</v>
       </c>
@@ -1852,7 +1855,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>128</v>
       </c>
@@ -1860,7 +1863,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="124" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>130</v>
       </c>
@@ -1868,7 +1871,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="124" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>132</v>
       </c>
@@ -1876,7 +1879,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="62" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>134</v>
       </c>
@@ -1884,7 +1887,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="93" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>136</v>
       </c>
@@ -1892,7 +1895,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="93" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>138</v>
       </c>
@@ -1900,7 +1903,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="217" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>140</v>
       </c>
@@ -1908,7 +1911,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="217" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>142</v>
       </c>
@@ -1916,7 +1919,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>144</v>
       </c>
@@ -1924,7 +1927,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>146</v>
       </c>
@@ -1932,7 +1935,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>148</v>
       </c>
@@ -1940,7 +1943,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="93" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>150</v>
       </c>
@@ -1948,7 +1951,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="93" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>152</v>
       </c>
@@ -1956,7 +1959,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="294.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>154</v>
       </c>
@@ -1964,7 +1967,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="93" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>156</v>
       </c>
@@ -1972,7 +1975,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>158</v>
       </c>
@@ -1980,7 +1983,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="62" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>160</v>
       </c>
@@ -1988,7 +1991,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="62" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>162</v>
       </c>
@@ -1996,7 +1999,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="93" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>164</v>
       </c>
@@ -2004,7 +2007,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="232.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>166</v>
       </c>
@@ -2012,7 +2015,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>168</v>
       </c>
@@ -2020,7 +2023,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="124" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>170</v>
       </c>
@@ -2028,7 +2031,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="93" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>172</v>
       </c>
@@ -2036,7 +2039,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>174</v>
       </c>
@@ -2044,7 +2047,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>176</v>
       </c>
@@ -2052,7 +2055,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="201.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>178</v>
       </c>
@@ -2060,7 +2063,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>180</v>
       </c>
@@ -2068,7 +2071,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="248" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>182</v>
       </c>
@@ -2076,7 +2079,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="124" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>184</v>
       </c>
@@ -2084,7 +2087,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>186</v>
       </c>
@@ -2092,7 +2095,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="62" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>188</v>
       </c>
@@ -2100,7 +2103,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>190</v>
       </c>
@@ -2108,7 +2111,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="93" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>192</v>
       </c>
@@ -2116,7 +2119,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>194</v>
       </c>
@@ -2124,7 +2127,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="170.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>196</v>
       </c>
@@ -2132,7 +2135,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="101" spans="1:2" ht="93" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>198</v>
       </c>
@@ -2140,7 +2143,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>200</v>
       </c>
@@ -2148,7 +2151,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="103" spans="1:2" ht="62" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>202</v>
       </c>
@@ -2156,7 +2159,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="62" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>204</v>
       </c>
@@ -2164,7 +2167,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="105" spans="1:2" ht="155" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>206</v>
       </c>
@@ -2172,7 +2175,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="93" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>208</v>
       </c>
@@ -2180,7 +2183,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="107" spans="1:2" ht="356.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>210</v>
       </c>
@@ -2188,7 +2191,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="108" spans="1:2" ht="263.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>212</v>
       </c>
@@ -2196,7 +2199,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="109" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>214</v>
       </c>
@@ -2204,7 +2207,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="110" spans="1:2" ht="248" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" ht="44.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>216</v>
       </c>

</xml_diff>